<commit_message>
remove recipes which contains allergy contents
</commit_message>
<xml_diff>
--- a/recipe.xlsx
+++ b/recipe.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="312">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -59,14 +59,14 @@
     <t>23 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For masala chawli
+    <t>, For masala chawli
 To make masala chawli, first prepare the mint paste by putting in a mixer, mint leaves, ginger, green chillies, lemon juice and 2 tbsp water. Grind to a smooth paste.
 Combine the soaked chawli, salt and 1 cup of water in a pressure cooker, mix well and pressure cook for 2 whistles.
 Allow the steam to escape before opening the lid. Do not discard the water. Keep aside.
 Heat the coconut oil or oil in a deep non-stick pan, add the onions and sauté on a medium flame for 1 to 2 minutes.
 Add the fresh tomato pulp, the dried fenugreek leaves, turmeric powder, a little salt, cooked chawli along with the water, mint paste and mix well.
 Cook on a medium flame for 4 to 5 minutes, while stirring occasionally.
-Serve masala chawli hot with bajra roti or roti.    </t>
+Serve masala chawli hot with bajra roti or roti.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -100,11 +100,11 @@
     <t>20 mins.</t>
   </si>
   <si>
-    <t xml:space="preserve">Clean and wash the moong dal.
+    <t>, Clean and wash the moong dal.
 Combine the moong dal, turai, onion, ginger-green chilli paste and turmeric powder with 2 cups of water and pressure cook for 2 to 3 whistles or until the dal is cooked.
 For the tempering, heat the oil in a non-stick pan, add the cumin seeds, asafoetida, chilli powder and garam masala and fry till the seeds crackle.
 Pour this tempering over the prepared dal. Add salt and simmer for 5 to 7 minutes.
-Serve hot, garnished with the coriander.    </t>
+Serve hot, garnished with the coriander.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -132,7 +132,7 @@
     <t>30 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For chana, tuvar and green moong dal
+    <t>, For chana, tuvar and green moong dal
 To make chana, tuvar and green moong dal, clean, wash and soak the dals in water about 30 minutes. Drain.
 Combine the soaked dals, salt and 3½ cups of water in a pressure cooker and pressure cook for 2 whistles.
 Allow the steam to escape before opening the lid. Keep aside.
@@ -142,7 +142,7 @@
 Add the dals and 2 cups of water, lemon juice and salt and simmer for 10 minutes.
 Serve the chana, tuvar and green moong dal hot garnished with the chopped coriander.
 Handy tip :
-To make a "jain" trevati dal, omit the onions, ginger and garlic and proceed as per the recipe.    </t>
+To make a "jain" trevati dal, omit the onions, ginger and garlic and proceed as per the recipe.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -158,61 +158,28 @@
     <t>https://www.tarladalal.com/chana-tuvar-and-green-moong-dal-trevati-dal-38470r</t>
   </si>
   <si>
-    <t>Recipe# 40603</t>
-  </si>
-  <si>
-    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 big brinjal (baingan / eggplant) slices    2 tsp chilli powder    1/2 tsp turmeric powder (haldi)    1 tbsp lemon juice    1/4 cup besan (bengal gram flour)    salt to taste    2 tsp oil for greasing and cooking    </t>
+    <t>Recipe# 5292</t>
+  </si>
+  <si>
+    <t>Dal Moghlai ( Low Cholesterol Recipe)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/4 cup toovar (arhar) dal    1/4 cup chana dal (split bengal gram)    1 cup chopped tomatoes    2 cups bottle gourd (doodhi / lauki) , cut into big pieces    1/4 tsp turmeric powder (haldi)    1 tsp cumin seeds (jeera)    1/2 tsp chopped garlic (lehsun)    1 tsp chopped green chillies    1 tsp grated ginger (adrak)    3/4 cup sliced onions    2 tsp oil    salt to taste    2 tbsp chopped coriander (dhania)    </t>
   </si>
   <si>
     <t>10 mins</t>
   </si>
   <si>
-    <t>20 mins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For baingan bhaja
-To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
-Add the baingan slices and mix well. Keep aside.
-Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
-Repeat step 3 to make 1 more batch.
-Serve the baingan bhaja immediately.    </t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 43 cal
-Protein 1.5 g
-Carbohydrates 4.6 g
-Fiber 3 g
-Fat 2.1 g
-Cholesterol 0 mg
-Sodium 4.3 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
-  </si>
-  <si>
-    <t>Recipe# 5292</t>
-  </si>
-  <si>
-    <t>Dal Moghlai ( Low Cholesterol Recipe)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3/4 cup toovar (arhar) dal    1/4 cup chana dal (split bengal gram)    1 cup chopped tomatoes    2 cups bottle gourd (doodhi / lauki) , cut into big pieces    1/4 tsp turmeric powder (haldi)    1 tsp cumin seeds (jeera)    1/2 tsp chopped garlic (lehsun)    1 tsp chopped green chillies    1 tsp grated ginger (adrak)    3/4 cup sliced onions    2 tsp oil    salt to taste    2 tbsp chopped coriander (dhania)    </t>
-  </si>
-  <si>
     <t>25 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For dal moghlai
+    <t>, For dal moghlai
 To make dal moghlai,clean, wash and soak the dals for about 30 minutes. Drain.
 Add the tomatoes, bottle gourd, turmeric powder, salt and 3 cups of water and pressure cook till the dals are tender.
 Heat the oil in a large non-stick pan and add the cumin seeds.
 When the seeds crackle, add the garlic, green chillies, ginger and onions and sauté till the onions turn golden brown in colour. Sprinkle about 1 tablespoon of water over it to prevent the onions from burning.
 Add the cooked dal mixture and 1 cup of water and bring to boil.
-Serve dal moghlai hot garnished with coriander.    </t>
+Serve dal moghlai hot garnished with coriander.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -240,12 +207,12 @@
     <t>1 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For moong sprouts
+    <t>, For moong sprouts
 To make healthy mung beans sprouts, combine the moong and enough water in a deep bowl, cover with a lid and keep aside to soak for 6 hours.
 Drain completely and tie them in a muslin cloth. Keep aside in a warm place to sprout for 10 to 12 hours.
 Combine the moong sprouts, 1¼ cups of water, salt and turmeric powder in a deep non-stick pan and mix well.
 Cover with a lid and cook on a medium flame for 15 minutes, while stirring occasionally.
-Use the healthy mung beans sprouts as required.    </t>
+Use the healthy mung beans sprouts as required.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per cup
@@ -270,14 +237,14 @@
     <t xml:space="preserve">1/2 cup yellow moong dal (split yellow gram)    1/2 cup quick cooking rolled oats    2 tbsp fresh curd (dahi)    3 tbsp grated onions    1/2 tsp finely chopped green chillies    2 tsp chaat masala    2 tsp chilli powder    1/4 tsp garam masala    1/4 tsp turmeric powder (haldi)    1 tsp ginger-garlic (adrak-lehsun) paste    2 tbsp finely chopped coriander (dhania)    salt to taste    2 tsp oil for greasing and cooking    healthy green chutney    </t>
   </si>
   <si>
-    <t xml:space="preserve">For oats moong dal tikki
+    <t>, For oats moong dal tikki
 To make oats moong dal tikki, clean, wash and boil the yellow moong dal in 1 cup of water in a deep pan till the dal is soft and cooked and all the water has evaporated.
 Drain and blend the dal in a mixer to a coarse paste.
 Transfer the paste into a bowl, add all the remaining ingredients and mix well.
 Divide the mixture into 12 equal portions and shape each portion into a 63 mm. (2½”) round flat tikki.
 Lightly grease a non-stick tava (griddle) with ½ tsp of oil.
 Cook each oats moong dal tikki, using 1/8 tsp of oil, till they turn golden brown in colour from both the sides. Evenly cooked from both the sides.
-Serve the oats moong dal tikki immediately with healthy green chutney.    </t>
+Serve the oats moong dal tikki immediately with healthy green chutney.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per tikki
@@ -305,11 +272,11 @@
     <t>3 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Heat the olive oil in a griller pan or a broad non-stick pan, add the zucchini and sauté on a medium flame for 1 minute.
+    <t>, Heat the olive oil in a griller pan or a broad non-stick pan, add the zucchini and sauté on a medium flame for 1 minute.
 Add the coloured capsicum and sauté on a medium flame for 1 minute.
 Add the mushroom and little sea salt and sauté on a medium flame for 1 minute.
 Cool put in a lunch box, along with other ingredients. It can be taken to work with a dressing in a separate small container.
-Just before eating, mix the dressing and toss well. Eat immediately.    </t>
+Just before eating, mix the dressing and toss well. Eat immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -334,11 +301,14 @@
     <t xml:space="preserve">3/4 cup brown rice    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">How to cook brown rice
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>, How to cook brown rice
 To cook brown rice, soak the brown rice in enough water for 30 minutes and drain well.
 Combine the brown rice along with 2 cups of water in a pressure cooker and pressure cook for 7 whistles.
 Allow the steam to escape before opening the lid.
-Separate each grain of the brown rice lightly with a fork. Use as required.    </t>
+Separate each grain of the brown rice lightly with a fork. Use as required.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per cup
@@ -366,13 +336,13 @@
     <t>0 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Beetroot juice in blender
+    <t>, Beetroot juice in blender
 Combine the beetroot cubes, carrots cubes, chopped parsley, chopped celery, black salt ( kala namak), 1 1/2 cups of water and 12 ice-cubes in a high quality blender jar (like vitamix) and blend well.
 Serve immediately.
 Mixer method
 This recipe doesn’t turn out good in a mixer jar because the texture of ingredients like carrots and beetroot are very hard.
 Handy tip:
-This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.    </t>
+This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per glass
@@ -397,13 +367,13 @@
     <t xml:space="preserve">3/4 cup masoor dal (split red lentil) , washed and drained    salt to taste    1 tbsp oil    1 tsp cumin seeds (jeera)    1/4 tsp asafoetida (hing)    1/2 cup finely chopped onions    6 curry leaves (kadi patta)    1 tsp garlic (lehsun) paste    1 cup chopped tomatoes    1 tsp chilli powder    1 tsp coriander (dhania) powder    1 tsp ginger-green chilli paste    1/2 tsp turmeric powder (haldi)    1/4 cup finely chopped coriander (dhania)    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine the masoor dal, little salt and 2 cups of water in a pressure cooker and pressure cook for 2 whistles.
+    <t>, Combine the masoor dal, little salt and 2 cups of water in a pressure cooker and pressure cook for 2 whistles.
 Allow the steam to escape before opening the lid. Keep aside.
 Heat the ghee in a deep non-stick pan and add the cumin seeds and asafoetida and sauté on a medium flame for 30 seconds.
 Add the onions, curry leaves and garlic paste and sauté on a medium flame for 1 minute.
 Add the tomatoes, chilli powder, coriander powder, ginger-green chilli paste, turmeric powder and salt, mix well and cook on a medium flame for 2 minutes ,while stirring occasionally.
 Add the cooked masoor dal, 1 cup of water and coriander, mix well and cook on a medium flame for 4 minutes, while stirring occasionally.
-Serve hot.    </t>
+Serve hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -419,35 +389,6 @@
     <t>https://www.tarladalal.com/masoor-dal-easy-masoor-dal-recipe-40586r</t>
   </si>
   <si>
-    <t>Recipe# 7468</t>
-  </si>
-  <si>
-    <t>Fenugreek and Mushroom Brown Rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 cups finely chopped fenugreek (methi) leaves    1 cup sliced mushrooms (khumbh)    1 cup brown rice    2 tsp oil    2 tsp finely chopped green chillies    1 tsp finely chopped ginger (adrak)    1 tbsp finely chopped garlic (lehsun)    1 cup finely chopped onions    1/2 cup finely chopped tomatoes    1/2 cup brinjal (baingan / eggplant) cubes    1/2 cup surti papdi seeds (fresh vaal seeds)    1/2 tsp chilli powder    salt to taste    2 tbsp finely chopped coriander (dhania)    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Heat the oil in a pressure cooker, add the green chillies, ginger, garlic, and onions and sauté on a medium flame for 2 minutes.
-Add the fenugreek leaves, mushrooms, tomatoes, brinjals, surti papadi seeds,and chilli powder, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
-Add the brown rice, 2¼ cups of hot water and salt, mix well and pressure cook for 4 whistles.
-Allow the steam to escape before opening the lid.
-Serve hot garnished with coriander.    </t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 151 cal
-Protein 3.9 g
-Carbohydrates 27.6 g
-Fiber 3.3 g
-Fat 2.8 g
-Cholesterol 0 mg
-Sodium 19.9 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/fenugreek-and-mushroom-brown-rice-7468r</t>
-  </si>
-  <si>
     <t>Recipe# 22173</t>
   </si>
   <si>
@@ -460,7 +401,7 @@
     <t>22 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Clean, wash and soak the urad dal in enough water in a bowl for 15 minutes. Drain well.
+    <t>, Clean, wash and soak the urad dal in enough water in a bowl for 15 minutes. Drain well.
 Combine the urad dal and 1½ cups of water in a pressure cooker, mix well and pressure cook for 3 whistles.
 Allow the steam to escape before opening the lid.
 Add the curds, 1½ cups of water, garlic paste, green chilli paste, salt and turmeric powder and mix well.
@@ -468,7 +409,7 @@
 Add the coriander and mix well.
 Serve hot.
 Handy tip:
-This dal tends to thicken if kept for too long. So, if you have made it in advance, add little water to it and re-heat it before serving.    </t>
+This dal tends to thicken if kept for too long. So, if you have made it in advance, add little water to it and re-heat it before serving.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -496,14 +437,14 @@
     <t>12 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For moong dal methi sabzi
+    <t>, For moong dal methi sabzi
 To make moong dal methi sabzi, wash and soak the yellow moong dal in enough water for 2 hours. Drain.
 Combine the soaked and drained moong dal and 5 tbsp of water in a deep pan, cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally. Keep aside.
 Heat the oil and add the cumin seeds.
 When they crackle, add the onions, garlic and green chillies and sauté for 1 minute.
 Add the fenugreek leaves, turmeric powder and salt and cook for 2 minutes.
 Add the soaked moong dal and 1 tbsp of water, mix well and cook on a medium flame for 1 minute.
-Serve moong dal methi sabzi hot with rotis.    </t>
+Serve moong dal methi sabzi hot with rotis.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -531,12 +472,12 @@
     <t>5 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For moong dal ki chaat
+    <t>, For moong dal ki chaat
 To make moong dal ki chaat, clean, wash and soak the moong dal in enough water for ½ hour and drain well.
 Combine 3 cups of water, moong dal and salt in a deep non-stick pan and cook it on a medium flame till it is half done, while stirring occasionally. Ensure that each grain of the dal is separate.
 Strain the dal using a strainer and keep aside to cool for 10 minutes.
 Combine all the ingredients, including the moong dal, in a large bowl and toss well.
-Serve the moong dal ki chaat immediately.    </t>
+Serve the moong dal ki chaat immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -561,13 +502,13 @@
     <t xml:space="preserve">2 cups watermelon (tarbuj) cubes    12 mm piece ginger (adrak) , finely chopped    1/2 tsp lemon juice    12 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">How to make ginger melon juice in a mixer
+    <t>, How to make ginger melon juice in a mixer
 To make ginger melon juice in a mixer, combine the watermelon, ginger, lemon juice and ice-cubes in a mixer jar and blend till smooth.
 Serve immediately.
 How to make in a juicer (hopper)
 To make ginger melon juice in a juicer (hopper), add watermelon cubes and ginger pieces a few at a time in the juicer / hopper.
 Add 6 ice-cubes in each of the 2 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per glass
@@ -595,14 +536,14 @@
     <t>2 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For oats idli
+    <t>, For oats idli
 To make oats idli, combine the oats and urad dal and blend in a mixer to a smooth powder.
 Add 1 cups of water, curd, ginger- green chilli paste and salt and mix well to make a batter of pouring consistency.
 Cover and keep aside to rest for 1 hour.
 Mix the batter well, add the fruit salt and 2 tsp of water and mix it gently.
 Grease the idli moulds using oil and put spoonfuls of batter into them.
 Steam in an idli steamer for 10 to 12 minutes or till they are cooked.
-Demould the oats idlis and serve idli immediately with sambhar.    </t>
+Demould the oats idlis and serve idli immediately with sambhar.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per idli
@@ -627,7 +568,7 @@
     <t xml:space="preserve">1/4 cup finely chopped zucchini (unpeeled)    1/4 cup finely chopped red capsicum    1/4 cup finely chopped yellow capsicum    1/4 cup finely chopped green capsicum    2 cups parboiled sprouted moong (whole green gram)    3/4 cup chopped apple (unpeeled and deseeded)    1 tbsp olive oil    2 tsp lemon juice    salt and to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine all the ingredients in a deep bowl and toss well. Serve immediately.    </t>
+    <t>, Combine all the ingredients in a deep bowl and toss well. Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -655,14 +596,14 @@
     <t>14 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For oats khichdi
+    <t>, For oats khichdi
 To make oats khichdi, heat the oil in a pressure cooker, add the green chilli paste, garlic paste and turmeric powder and sauté on a medium flame for a few seconds.
 Add the oats and yellow moong dal and sauté on a medium flame for 2 to 3 minutes
 Add 2 cups of hot water and salt, mix well and pressure cook for 2 whistles.
 Allow the steam to escape before opening the lid.
 Serve oats khichdi immediately with low-fat curds.
 Handy tip:
-Serving this oats khichdi immediately is important to avoid it being lumpy and sticky.    </t>
+Serving this oats khichdi immediately is important to avoid it being lumpy and sticky.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -687,7 +628,7 @@
     <t xml:space="preserve">3/4 cup masoor (split red lentil) dal    1/4 tsp turmeric powder (haldi)    1/4 tsp salt    1 1/2 tsp oil    1/2 tsp cumin seeds (jeera)    1 tsp finely chopped ginger (adrak)    1/4 cup chopped onions    1/4 tsp garlic (lehsun) paste    1/4 tsp garam masala    1/4 tsp chilli powder    1/4 tsp asafoetida (hing)    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine the masoor dal, turmeric powder, salt and 1 cup of water in a pressure cooker, mix well and pressure cook for 3 whistles.
+    <t>, Combine the masoor dal, turmeric powder, salt and 1 cup of water in a pressure cooker, mix well and pressure cook for 3 whistles.
 Allow the steam to escape before opening the lid.
 Add 2½ cups of water and whisk it well using a whisk till smooth. Keep aside.
 Heat the oil in a deep non-stick pan add the cumin seeds and ginger and sauté on a medium flame for few seconds.
@@ -695,7 +636,7 @@
 Lower the flame add the garlic paste, garam masala, chilli powder, asafoetida and 1 tbsp water and sauté for few seconds.
 Add the whisked dal water mixture, mix well and cook on a medium flame for 2 to 3 minute, while stirring occasionally.
 Switch off the flame, add the lemon juice and mix well.
-Serve hot.    </t>
+Serve hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -720,14 +661,14 @@
     <t xml:space="preserve">2 cups mushrooms (khumbh)    1 medium red capsicum    1 medium green capsicum    1 medium yellow capsicum    1 tsp dried rosemary or dried mixed herbs    1/2 tsp dried thyme    1 1/2 tsp lemon juice    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Wash, clean and dry the mushrooms and place them on a baking tray and bake in a pre-heated oven at 200°c (400°f) for 11 minutes or till the mushrooms turn light brown in colour, while turning them once after 6 minutes. Keep aside to cool slightly.
+    <t>, Wash, clean and dry the mushrooms and place them on a baking tray and bake in a pre-heated oven at 200°c (400°f) for 11 minutes or till the mushrooms turn light brown in colour, while turning them once after 6 minutes. Keep aside to cool slightly.
 Once they are slightly cooled, cut the stems of the mushrooms and discard them.
 Cut the mushrooms into cubes and keep aside.
 Pierce the red capsicum with a fork and roast it over an open flame till it turns black from all the sides.
 Cool, wash it in cold water and remove the burnt skin, stem and seeds and discard them. Cut the capsicum into cubes and keep aside.
 Repeat steps 4 and 5 for green and yellow capsicum.
 Combine the mushroom and capsicum cubes in a deep bowl, add the rosemary, thyme, lemon juice and salt and toss well.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -752,7 +693,7 @@
     <t xml:space="preserve">3/4 cup peeled carrot cubes    3/4 cup red capscium cubes    1 cup deseeded tomato cubes , see handy tip    10 to 12 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">Carrot and red pepper juice in vitamix
+    <t>, Carrot and red pepper juice in vitamix
 Combine the carrots cubes, capsicum cubes, tomato cubes, ½ cup of water and ice-cubes in a high quality blender jar (like vitamix) and blend well.
 Serve immediately.
 Carrot and red pepper juice in juicer (hopper)
@@ -760,7 +701,7 @@
 Add 2 to 3 ice-cubes in each of the 4 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
 Serve immediately.
 Handy tip:
-2 tomatoes will give approx. 1 cup of deseeded tomato cubes.    </t>
+2 tomatoes will give approx. 1 cup of deseeded tomato cubes.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per small glass
@@ -785,7 +726,7 @@
     <t xml:space="preserve">1 cup red capscium cubes    1 cup peeled carrot cubes    1 cup apple cubes    10 to 12 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">Red capsicum, carrot and apple juice in vitamix
+    <t>, Red capsicum, carrot and apple juice in vitamix
 To make red capsicum, carrot and apple juice, combine the red capsicum cubes, carrot cubes, apple cubes, 1 cup of water and ice cubes in a high quality blender jar (like vitamix) and blend well till smooth and frothy.
 Serve immediately.
 Red capsicum, carrot and apple juice in juicer
@@ -793,7 +734,7 @@
 Add 5 to 6 ice-cubes in each of the 2 glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
 Serve the red capsicum, carrot and apple juice immediately.
 Handy tip:
-This recipe makes use of unpeeled apples, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.    </t>
+This recipe makes use of unpeeled apples, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per small glass
@@ -818,13 +759,13 @@
     <t xml:space="preserve">2 cups carrot peeled and cut into thick strips    1 1/4 cups unpeeled apple wedges    1/2 tsp roughly chopped ginger (adrak)    10 to 12 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">Apple carrot juice in blender
+    <t>, Apple carrot juice in blender
 Combine the carrots cubes, apple cubes, ginger (adrak),1 cup of water and 10 to 12 ice-cubes in a high quality blender jar (like vitamix) and blend well.
 Serve immediately.
 Apple carrot juice in juicer
 Add the carrot cubes, apple cubes and ginger a few at a time in a juicer (hopper).
 Add 2 to 3 ice-cubes in each of the 4 small glasses or 2 big glasses and pour equal quantities of juice over it. Note that some amount of fiber will be lost while making juice in a juicer.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per glass
@@ -849,11 +790,11 @@
     <t xml:space="preserve">1/4 cup finely chopped mint leaves (phudina)    3 cups apple cubes    1 tsp lemon juice    1 tsp ginger (adrak) juice , refer handy tip    1 tsp honey    salt and to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">For minty apple salad
+    <t>, For minty apple salad
 Combine all the ingredients in a deep bowl and toss well.
 Serve the minty apple salad immediately.
 Handy tip:
-2 tbsp of grated ginger when placed in a muslin cloth and squeezed gives 2 tsp of ginger juice.    </t>
+2 tbsp of grated ginger when placed in a muslin cloth and squeezed gives 2 tsp of ginger juice.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -878,12 +819,12 @@
     <t xml:space="preserve">1/2 cup cucumber cubes    3/4 cup chana dal (split bengal gram)    1 tsp cumin seeds (jeera)    1 tsp green chilli paste    a pinch of turmeric powder (haldi)    1/2 tsp chilli powder    1 tbsp oil    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">For dry masala chana dal
+    <t>, For dry masala chana dal
 To make dry masala chana dal, wash and soak the chana dal in enough hot water in a deep bowl for 1 hour. Drain and keep aside.
 Heat the oil in a deep non-stick pan, add the cumin seeds and sauté on a medium flame for 30 seconds.
 Add the soaked chana dal, green chilli paste, turmeric powder, chilli powder and ¼ cup water, mix well and cover and cook on a medium flame for 6 minutes, while stirring occasionally.
 Add the cucumber, salt and more ¼ cup water, mix well and cover and cook on a medium flame for 3 minutes, while stirring occasionally.
-Serve the dry masala chana dal hot.    </t>
+Serve the dry masala chana dal hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -908,7 +849,7 @@
     <t xml:space="preserve">1/4 cup finely chopped onions    1/2 cup grated carrot    1/4 cup grated beetroot    1/4 cup boiled and mashed potatoes    1/2 tsp fennel seeds (saunf)    1/2 tsp cumin seeds (jeera)    1/2 tsp coriander (dhania) seeds    1 tsp oil    1/2 tsp ginger (adrak) paste    1 tsp finely chopped green chillies    1/2 tsp chilli powder    1/4 tsp dried mango powder (amchur)    1/4 tsp salt    1/4 tsp freshly ground black pepper (kalimirch)    1 tsp oil brush (for greasing) and cooking    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine the fennel seeds, cumin seeds and coriander seeds in a mortal pestle (khalbatta) till coarse. Keep aside.
+    <t>, Combine the fennel seeds, cumin seeds and coriander seeds in a mortal pestle (khalbatta) till coarse. Keep aside.
 Heat the oil in a broad non-stick pan, add the ginger paste and green chillies and sauté on a medium flame for 30 seconds.
 Add the onions and sauté on a medium flame for 1 minute.
 Add the carrot and beetroot and sauté on a medium flame for 1 minute.
@@ -917,7 +858,7 @@
 Divide the mixture into 12 equal portions and roll each portion into an oblong shape.
 Heat a non-stick tava (griddle) and grease it using the remaining ½ tsp of oil.
 Place the chops on it and cook using ½ tsp of oil till they turn golden brown in colour from both the sides.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per chop
@@ -942,13 +883,13 @@
     <t xml:space="preserve">1 1/2 cups sprouted matki (moath beans)    1/4 cup besan (bengal gram flour)    1/4 cup finely chopped coriander (dhania)    1/4 cup chopped tomatoes    1/4 cup grated carrot    2 tsp ginger-green chilli paste    1/4 tsp cumin seeds (jeera)    1/4 tsp asafoetida (hing)    salt to taste    2 tsp oil for greasing and cooking    </t>
   </si>
   <si>
-    <t xml:space="preserve">For sprouted matki uttapam
+    <t>, For sprouted matki uttapam
 To make sprouted matki uttapam, combine the sprouted matki and ½ cup of water in a mixer and blend till smooth.
 Transfer the mixture into a deep bowl, add besan, coriander, tomatoes, carrot, ginger-green chilli paste, cumin seeds, hing, salt and mix well.
 Grease a non-stick pan with ¼ tsp of oil.
 Pour a ladleful of the batter and spread in a circular motion to make a 125 mm. (5") diameter thick circle.
 Cook till they turn brown in colour from both the sides using a little oil.
-Serve the sprouted matki uttapam immediately with coconut chutney.    </t>
+Serve the sprouted matki uttapam immediately with coconut chutney.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per uttapam
@@ -973,13 +914,13 @@
     <t xml:space="preserve">1/2 cup powered quick cooking rolled oats    1/2 cup finely chopped spring onions whites and greens    1/2 cup urad dal (split black lentils)    2 tsp crushed black pepper (kalimirch)    salt to taste    2 tsp oil for greasing and cooking    </t>
   </si>
   <si>
-    <t xml:space="preserve">For oats appe
+    <t>, For oats appe
 To make oats appe, soak the urad dal in enough water in a deep bowl and keep aside to soak for 1 hour. Drain well.
 Blend the urad dal in a mixer using ¼ cup of water till smooth.
 Transfer the mixture into a deep bowl, add the oats, spring onions, crushed black pepper and salt and mix very well.
 Heat an appe mould on a medium flame and grease it using ¼ tsp of oil. Pour 1 tbsp of the batter into each mould and cook using ¼ tsp of oil till the lower surface becomes golden brown and then turn each appe upside down using a fork so as to cook them from the other side as well.
 Repeat step 4 to make more appes.
-Serve the oats appe immediately.    </t>
+Serve the oats appe immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per appe
@@ -1004,12 +945,12 @@
     <t xml:space="preserve">1 cup besan (bengal gram flour)    1/4 cup fresh tomato pulp    1/4 tsp asafoetida (hing)    1/4 tsp turmeric powder (haldi)    1 1/2 tsp chilli powder    1/4 tsp freshly ground black pepper (kalimirch)    1 tsp oil    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">For baked masala sev
+    <t>, For baked masala sev
 To make baked masala sev combine gram flour, tomato pulp, hing, haldi, chilli powder, salt, pepper and oil in a deep bowl, mix well and knead into a soft dough without using any water.
 Shape the dough into a cylindrical roll, fill the dough into the “sev press” and press out strands onto a greased baking tray.
 Bake in a preheated oven at 200°c (400°f) for 14 minutes, turn them over after 9 minutes then break into pieces and bake again for 5 minutes, while tossing twice in between.
 Cool, break them into pieces.
-Store baked masala sev in an air-tight container and use as required.    </t>
+Store baked masala sev in an air-tight container and use as required.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per tablespoon
@@ -1037,11 +978,11 @@
     <t>18 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For minty quinoa for ibs
+    <t>, For minty quinoa for ibs
 To make minty quinoa heat oil in a deep non-stick pan, add the carrots, celery and green chillies sauté on a medium flame for 2 minutes.
 Add the quinoa, red pumpkin, bayleaves, salt, pepper powder and 2½ cups of water and mix well. Cover with a lid and cook on a slow flame for 15 to 16 minutes, while stirring occasionally.
 Add the mint leaves and mix well.
-Serve minty quinoa immediately.    </t>
+Serve minty quinoa immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1066,13 +1007,13 @@
     <t xml:space="preserve">1/2 cup quick cooking rolled oats    3/4 cup brown rice    2 tbsp yellow moong dal (split yellow gram) , washed and drained    2 tsp oil    1/2 cup finely chopped onions    1 tsp garlic (lehsun) paste    1/2 tsp ginger (adrak) paste    1/4 cup chopped french beans    1/4 cup chopped carrot    1/4 cup green peas    1/2 tsp chilli powder    1/2 tsp garam masala    2 tbsp finely chopped coriander (dhania)    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Clean, wash and soak the brown rice in enough water in a deep bowl for 30 minutes. Drain well and keep aside.
+    <t>, Clean, wash and soak the brown rice in enough water in a deep bowl for 30 minutes. Drain well and keep aside.
 Heat the oil in a pressure cooker, add the onions, garlic paste and ginger paste and sauté on a medium flame for 1 minute.
 Add the french beans, carrot, green peas, chilli powder and garam masala and sauté on a medium flame for 1 minute.
 Add the brown rice, yellow moong dal, oats, coriander and salt, mix well and cook on a medium flame for 2 minutes, while stirring continuously.
 Add 3 cups of hot water, mix well and pressure cook for 7 whistles.
 Allow the steam to escape before opening the lid.
-Serve hot.    </t>
+Serve hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1097,8 +1038,8 @@
     <t xml:space="preserve">1 1/2 cups sliced avocados    1 cup deseeded and sliced tomatoes    1 tbsp olive oil    1/2 tsp mustard (rai / sarson) powder    1 tsp lemon juice    salt and to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine all the ingredients along with the dressing in a deep bowl and toss well.
-Serve immediately.    </t>
+    <t>, Combine all the ingredients along with the dressing in a deep bowl and toss well.
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1123,9 +1064,9 @@
     <t xml:space="preserve">2 cups bean sprouts    1/4 cup finely chopped dill leaves    1/2 cup chopped tomatoes    1 tbsp lemon juice    1/4 cup chopped basil    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">For bean sprouts and suva tossed salad
+    <t>, For bean sprouts and suva tossed salad
 To make bean sprouts and suva tossed salad, combine all the ingredients in a deep bowl and toss well.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1153,12 +1094,12 @@
     <t>16 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">For gavarfali ki sukhi subzi
+    <t>, For gavarfali ki sukhi subzi
 To make gavarfali ki sukhi sabzi, heat the oil in a broad non-stick pan and add the cumin seeds.
 When the seeds crackle, add the onions, garlic paste and turmeric powder and sauté on a medium flame for 2 minutes.
 Add the cluster beans, salt and ½ cup of water and mix well. Cover with a lid and cook on a medium flame for 8 to 10 minutes, while stirring occasionally.
 Add the coriander-cumin seeds powder, chilli powder and 1 tbsp of water, mix well. Cover with a lid and again cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
-Serve the gavarfali ki sukhi sabzi hot.    </t>
+Serve the gavarfali ki sukhi sabzi hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1183,9 +1124,9 @@
     <t xml:space="preserve">2 cups chilled and roughly chopped muskmelon (kharbooja)    4 cups chilled and roughly chopped pineapple    8 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">Add the muskmelon and pineapple a few at a time in a hopper.
+    <t>, Add the muskmelon and pineapple a few at a time in a hopper.
 Pour equal quantities of the juice into 4 individual glasses.
-Serve immediately topped with 2 ice-cubes in each glass.    </t>
+Serve immediately topped with 2 ice-cubes in each glass.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per small glass
@@ -1210,7 +1151,7 @@
     <t xml:space="preserve">3 cups apple cubes    2 tsp lemon juice    crushed ice for serving , optional    </t>
   </si>
   <si>
-    <t xml:space="preserve">Juicer method
+    <t>, Juicer method
 Add the apple cubes a few at a time in the juicer.
 Add the lemon juice and mix well.
 Add some crushed ice in 2 individual glasses and pour equal quantities of the juice over it.
@@ -1218,7 +1159,7 @@
 Mixer method
 This recipe doesn’t turn out good in a mixer because the texture of ingredients like apple is very hard.
 Handy tip:
-This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.    </t>
+This recipe makes use of unpeeled fruits and vegetables, hence take care to clean and wash them well before chopping, to get rid of dirt, germs and chemical residues.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per small glass
@@ -1234,40 +1175,6 @@
     <t>https://www.tarladalal.com/apple-magic-lemony-apple-juice-6213r</t>
   </si>
   <si>
-    <t>Recipe# 22206</t>
-  </si>
-  <si>
-    <t>Bhindi Masala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 tender ladies finger (bhindi)    2 tbsp besan (bengal gram flour)    2 tsp oil    1/2 cup roughly chopped onions    1 cup chopped coriander (dhania)    2 tsp ginger-green chilli paste    1/2 tsp turmeric powder (haldi)    1 tbsp coriander-cumin seeds (dhania-jeera) powder    1 tsp garam masala    2 tsp roasted sesame seeds (til)    1 tbsp lemon juice    salt to taste    rotis/parathas    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For the bhindi masala paste
-Combine all the ingredients and 2 tbsp of water in a mixer and blend till smooth.
-Transfer the mixture into a deep bowl, add the besan and mix well. Keep aside.
-How to proceed to make bhindi masala
-To make bhindi masala, wash, dry and slit the bhindi lengthwise.
-Stuff each bhindi with a little prepared paste. Keep the remaining paste aside.
-Heat a non-stick tava (griddle), put the remaining paste and 2 tbsp of water and sauté on a medium flame for 2 minutes.
-Add the stuffed bhindis and sauté on a medium flame for 4 minutes.
-Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
-Serve the bhindi masala hot with rotis or parathas.    </t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per serving
-Energy 83 cal
-Protein 3.6 g
-Carbohydrates 14.2 g
-Fiber 3.6 g
-Fat 1.4 g
-Cholesterol 0 mg
-Sodium 15.7 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/bhindi-masala-22206r</t>
-  </si>
-  <si>
     <t>Recipe# 8651</t>
   </si>
   <si>
@@ -1277,8 +1184,8 @@
     <t xml:space="preserve">1 cup mashed ripe avocado    1 tsp lemon juice    2 tbsp chopped tomatoes    1/2 tsp chopped green chillies    salt to taste    corn chips    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine all the ingredients in a deep bowl and mix well.
-Serve with corn chips.    </t>
+    <t>, Combine all the ingredients in a deep bowl and mix well.
+Serve with corn chips.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per tbsp
@@ -1294,36 +1201,6 @@
     <t>https://www.tarladalal.com/avocado-dip-avocado-jain-dip-8651r</t>
   </si>
   <si>
-    <t>Recipe# 38954</t>
-  </si>
-  <si>
-    <t>Fluffy Egg White Masala Omelette</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 eggs whites    1 tsp olive oil    salt and freshly ground to taste    1/4 cup finely chopped onions    1/2 cup red and yellow capsicum chopped    1/4 cup finely chopped mushrooms (khumbh)    1/4 cup finely chopped tomatoes    1/2 tsp finely chopped green chillies    1 tsp olive oil    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">For the masala vegetables
-In a pan, heat the olive oil and sauté the onions, capsicums , mushrooms, and green chilli for 1 minute. Add the tomatoes and cook again. Keep aside.
-How to proceed
-Beat the egg whites in a electric beater on a slow for 2 to 3 minutes or until the mixture is thick and frothy.
-Heat the olive oil in a 10 inch pan. Add the beaten egg and cook for a few minutes checking with a spatula to see when the bottom of the egg is done. Then add the cooked masala vegetables in the centre of the omelette. Fold the omelette into half and serve hot with a whole wheat toast.
-Sprinkle fresh pepper on top.    </t>
-  </si>
-  <si>
-    <t>Nutrient values (Abbrv) per omeleltte
-Energy 394 cal
-Protein 22 g
-Carbohydrates 8.9 g
-Fiber 2.6 g
-Fat 30.3 g
-Cholesterol 0 mg
-Sodium 9.4 mg</t>
-  </si>
-  <si>
-    <t>https://www.tarladalal.com/fluffy-egg-white-masala-omelette-38954r</t>
-  </si>
-  <si>
     <t>Recipe# 39688</t>
   </si>
   <si>
@@ -1333,9 +1210,9 @@
     <t xml:space="preserve">5 cups mushroom (khumbh) halves    1 cup capsicum cubes    2 tsp oil    salt to taste    4 whole dry kashmiri red chillies , broken into pieces    6 garlic (lehsun) cloves    1/2 cup roughly chopped onions    </t>
   </si>
   <si>
-    <t xml:space="preserve">Heat the oil in a broad non-stick pan, add the prepared paste and 2 tbsp of water, mix well and cook on a medium flame for 2 minutes, while stirring occasionally.
+    <t>, Heat the oil in a broad non-stick pan, add the prepared paste and 2 tbsp of water, mix well and cook on a medium flame for 2 minutes, while stirring occasionally.
 Add the capsicum cubes, mushrooms and salt and mix well. Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1363,7 +1240,7 @@
     <t>28 mins</t>
   </si>
   <si>
-    <t xml:space="preserve">Combine the masoor dal and 1½ cups of water in a pressure cooker and pressure cook for 3 whistles.
+    <t>, Combine the masoor dal and 1½ cups of water in a pressure cooker and pressure cook for 3 whistles.
 Allow the steam to escape before opening the lid.
 Add 1½ cups of water and mix well using a whisk. Keep aside.
 Heat the oil in a deep non-stick pan and add the cumin seeds and asafoetida and sauté on a medium flame for a few seconds.
@@ -1371,7 +1248,7 @@
 Add the tomatoes, mix well and cook on a medium flame for 1 minute.
 Add the cluster beans, chilli powder, turmeric powder, salt and ½ cup of water and mix well. Cover with a lid and cook on a medium flame for 6 minutes, while stirring occasionally.
 Add the cooked masoor dal, mix well and cook on a medium flame for another 3 minutes, while stirring occasionally.
-Serve hot.    </t>
+Serve hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1396,14 +1273,14 @@
     <t xml:space="preserve">1/2 cup toovar (arhar) dal    1/4 cup yellow moong dal (split yellow gram)    1/2 cup chana dal (split bengal gram)    1 cup chopped fenugreek leaves (methi)    2 cups chopped coriander (dhania)    1/4 cup boiled green peas    1/4 cup grated coconut    2 tsp chopped green chillies    1/4 cup chopped onions    1/4 cup grated carrot    salt to taste    oil for greasing    </t>
   </si>
   <si>
-    <t xml:space="preserve">For dal and vegetable idli
+    <t>, For dal and vegetable idli
 To make dal and vegetable idli, wash and soak the dals together at least 3 hours.
 Drain, add water and grind to a smooth paste.
 Add the fenugreek, coriander, green peas, coconut, green chillies, onion, carrot and salt and mix well.
 Gradually add water as required to make a thick batter. We added a total of 3/4th cup water.
 Just before steaming, add fruit salt and 1 tbsp of water to the batter and mix gently.
 Pour into greased idli moulds and steam for 10 to 12 minutes till done.
-Serve the dal and vegetable idli hot with sambhar and coconut chutney.    </t>
+Serve the dal and vegetable idli hot with sambhar and coconut chutney.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per idli
@@ -1428,11 +1305,11 @@
     <t xml:space="preserve">1/2 cup whole masoor (whole red lentil)    salt to taste    1/2 cup deseeded and chopped cucumber    1/2 cup chopped carrot    1/4 cup deseeded and chopped tomatoes    1/2 cup chopped spring onions (whites and greens)    1/2 tbsp olive oil    1 tsp lemon juice    1/2 tsp finely chopped green chillies    1/4 tsp freshly ground black pepper (kalimirch)    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Clean, wash and soak the whole masoor in a deep bowl in enough water overnight. Drain well.
+    <t>, Clean, wash and soak the whole masoor in a deep bowl in enough water overnight. Drain well.
 Combine the whole soaked masoor, salt and ½ cup of water in a deep non-stick pan and mix well. Cover with a lid and cook on a medium flame for 8 minutes or till all the water has been evaporated, while stirring occasionally. Keep aside to cool completely.
 Once cooled, transfer the cooked whole masoor into a deep bowl, add all the remaining ingredients and mix well.
 Finally, pour the prepared dressing over it and toss gently.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1457,13 +1334,13 @@
     <t xml:space="preserve">1/4 cup rajma (kidney beans)    1/4 cup chana dal (split bengal gram)    1/2 cup chilkewali urad dal (spit black gram with skin)    salt to taste    2 tsp oil    1 tbsp finely chopped garlic (lehsun)    1/2 cup finely chopped onions    1 tsp green chilli paste    1 cup finely chopped tomatoes    1 tsp chilli powder    2 tsp cumin seeds (jeera) powder    1/4 cup chopped coriander (dhania)    1 tbsp lemon juice    </t>
   </si>
   <si>
-    <t xml:space="preserve">Clean, wash and soak the rajma, chana and urad dal in a deep bowl with enough water overnight.
+    <t>, Clean, wash and soak the rajma, chana and urad dal in a deep bowl with enough water overnight.
 Drain the soaked dals, add 4 cups water and salt, mix well and pressure cook for 4 whistles.
 Allow the steam to escape before opening the lid. Keep aside.
 Heat the oil in a deep non-stick pan, add the garlic, onions and green chilli paste and sauté on a medium flame for 1 minute.
 Add the tomatoes, chilli powder, cumin seeds powder, little salt and 2 tbsp of water, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
 Add the cooked dals and coriander, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.
-Add the lemon juice, mix well and serve hot.    </t>
+Add the lemon juice, mix well and serve hot.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1488,9 +1365,9 @@
     <t xml:space="preserve">1 1/2 cups chilled muskmelon (kharbooja) cubes    3/4 cup chilled pear cubes    3/4 cup chilled apple cubes    1/4 cup finely chopped parsley    1/2 cup thick low-fat curds (dahi)    1/4 tsp mustard (rai / sarson) powder    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine the muskmelon, pear and apples in a deep bowl and mix well.
+    <t>, Combine the muskmelon, pear and apples in a deep bowl and mix well.
 Just before serving, add the parsley dressing and toss well.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1515,11 +1392,11 @@
     <t xml:space="preserve">2 cups watermelon (tarbuj) cubes    1/2 cup orange segments    1/2 cup sweet lime (mosambi) segments    1/2 cup pomegranate (anar)    2 tsp extra virgin olive oil    2 tbsp finely chopped parsley    1 tsp lemon juice    1/2 tsp sea salt (khada namak)    </t>
   </si>
   <si>
-    <t xml:space="preserve">For citrus watermelon salad
+    <t>, For citrus watermelon salad
 To make citrus watermelon salad, prepare the parsley lemon extra virgin olive oil dressing by mixing all ingredients.
 In a deep bowl put watermelon (tarbuj) cubes, orange segments, sweet lime (mosambi) segments and pomegranate (anar).
 Add the dressing just before serving. Toss well.
-Serve citrus watermelon salad immediately.    </t>
+Serve citrus watermelon salad immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1544,11 +1421,11 @@
     <t xml:space="preserve">2 1/4 cups mixed boiled beans (rajma , chawli and chick peas)    1/2 cup sliced spring onions    1/2 cup tomato cubes    1 tsp finely chopped green chillies    1 tbsp finely chopped coriander (dhania)    2 tbsp lemon juice    2 tsp chaat masala    1/4 tsp black salt (sanchal)    salt and to taste    1 tbsp finely chopped coriander (dhania)    </t>
   </si>
   <si>
-    <t xml:space="preserve">For chawli, rajma and chick pea salad
+    <t>, For chawli, rajma and chick pea salad
 To make chawli, rajma and chick pea salad, combine all the ingredients (except the dressing) in a deep bowl and mix well.
 Refrigerate for 1 hour or longer.
 Just before serving add the peppy lemon dressing. Toss well.
-Serve healthy three bean chaat salad chilled garnished with coriander.    </t>
+Serve healthy three bean chaat salad chilled garnished with coriander.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1573,11 +1450,11 @@
     <t xml:space="preserve">1 cup papaya cubes    1/4 cup coconut meat (nariyal ki malai)    3/4 cup chilled coconut water (nariyal ka pani)    10 to 12 ice-cubes    </t>
   </si>
   <si>
-    <t xml:space="preserve">For papaya coconut drink
+    <t>, For papaya coconut drink
 To make papaya coconut drink, combine the papaya cubes, coconut meat, coconut water and ice cubes in a mixer jar and blend well till smooth.
 Serve the papaya coconut drinkimmediately.
 Handy tip:
-This recipe doesn’t turn out good in a juicer (hopper) because the texture of papaya is very soft.    </t>
+This recipe doesn’t turn out good in a juicer (hopper) because the texture of papaya is very soft.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per glass
@@ -1602,10 +1479,10 @@
     <t xml:space="preserve">2 tbsp finely chopped mint leaves (phudina)    1 1/2 cups soaked and cooked chawli , refer handy tip    1/2 cup chopped cucumber    1/2 cup finely chopped onions    1/2 cup finely chopped tomatoes    2 tbsp finely chopped coriander (dhania)    1/2 tsp finely chopped green chillies    1/4 tsp black salt (sanchal)    1/2 tbsp lemon juice    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine all the ingredients in a bowl and toss well.
+    <t>, Combine all the ingredients in a bowl and toss well.
 Serve immediately or refrigerate for 1 hour and serve chilled.
 Handy tip:
-½ cup of raw chawli, when soaked and boiled yields 1½ cups cooked chawli. Ensure not to overcook the chawli for this recipe.    </t>
+½ cup of raw chawli, when soaked and boiled yields 1½ cups cooked chawli. Ensure not to overcook the chawli for this recipe.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1630,9 +1507,9 @@
     <t xml:space="preserve">1 cup thinly sliced carrot    1 cup thinly sliced cucumber    1/2 cup soaked and boiled rajma (kidney beans)    1/2 cup sliced spring onions (white and greens)    2 tbsp finely chopped mint leaves (phudina)    4 tsp honey    1 tbsp lemon juice    salt to taste    </t>
   </si>
   <si>
-    <t xml:space="preserve">Combine all the ingredients for the salad in a bowl, toss well and refrigerate for at least 1 hour.
+    <t>, Combine all the ingredients for the salad in a bowl, toss well and refrigerate for at least 1 hour.
 Just before serving, add the mint dressing and toss well.
-Serve immediately.    </t>
+Serve immediately.</t>
   </si>
   <si>
     <t>Nutrient values (Abbrv) per serving
@@ -1690,7 +1567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1885,10 +1762,10 @@
         <v>44</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>46</v>
@@ -1920,45 +1797,45 @@
         <v>51</v>
       </c>
       <c r="F7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="G7" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="H7" t="s" s="0">
+      <c r="I7" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="I7" t="s" s="0">
+      <c r="J7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K7" t="s" s="0">
         <v>54</v>
-      </c>
-      <c r="J7" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K7" t="s" s="0">
-        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s" s="0">
         <v>56</v>
       </c>
-      <c r="B8" t="s" s="0">
+      <c r="C8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="C8" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s" s="0">
+      <c r="F8" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>58</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>45</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>59</v>
@@ -1990,7 +1867,7 @@
         <v>64</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>65</v>
@@ -2025,30 +1902,30 @@
         <v>71</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C11" t="s" s="0">
         <v>2</v>
@@ -2057,13 +1934,13 @@
         <v>3</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>79</v>
@@ -2095,30 +1972,30 @@
         <v>84</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>38</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J12" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s" s="0">
         <v>2</v>
@@ -2127,33 +2004,33 @@
         <v>3</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="J13" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s" s="0">
         <v>2</v>
@@ -2162,33 +2039,33 @@
         <v>3</v>
       </c>
       <c r="E14" t="s" s="0">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F14" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G14" t="s" s="0">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s" s="0">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="I14" t="s" s="0">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J14" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K14" t="s" s="0">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C15" t="s" s="0">
         <v>2</v>
@@ -2197,33 +2074,33 @@
         <v>3</v>
       </c>
       <c r="E15" t="s" s="0">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>37</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="H15" t="s" s="0">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I15" t="s" s="0">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J15" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K15" t="s" s="0">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" t="s" s="0">
         <v>2</v>
@@ -2232,33 +2109,33 @@
         <v>3</v>
       </c>
       <c r="E16" t="s" s="0">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F16" t="s" s="0">
+        <v>112</v>
+      </c>
+      <c r="G16" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="G16" t="s" s="0">
-        <v>111</v>
-      </c>
       <c r="H16" t="s" s="0">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="I16" t="s" s="0">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J16" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K16" t="s" s="0">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s" s="0">
         <v>2</v>
@@ -2267,33 +2144,33 @@
         <v>3</v>
       </c>
       <c r="E17" t="s" s="0">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F17" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G17" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H17" t="s" s="0">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I17" t="s" s="0">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J17" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K17" t="s" s="0">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s" s="0">
         <v>2</v>
@@ -2302,33 +2179,33 @@
         <v>3</v>
       </c>
       <c r="E18" t="s" s="0">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F18" t="s" s="0">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="G18" t="s" s="0">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="H18" t="s" s="0">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I18" t="s" s="0">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J18" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K18" t="s" s="0">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s" s="0">
         <v>2</v>
@@ -2337,33 +2214,33 @@
         <v>3</v>
       </c>
       <c r="E19" t="s" s="0">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F19" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G19" t="s" s="0">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="H19" t="s" s="0">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s" s="0">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J19" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K19" t="s" s="0">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C20" t="s" s="0">
         <v>2</v>
@@ -2372,13 +2249,13 @@
         <v>3</v>
       </c>
       <c r="E20" t="s" s="0">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s" s="0">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s" s="0">
-        <v>137</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s" s="0">
         <v>138</v>
@@ -2410,10 +2287,10 @@
         <v>143</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="H21" t="s" s="0">
         <v>144</v>
@@ -2445,10 +2322,10 @@
         <v>149</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s" s="0">
         <v>150</v>
@@ -2480,10 +2357,10 @@
         <v>155</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>111</v>
+        <v>13</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s" s="0">
         <v>156</v>
@@ -2515,10 +2392,10 @@
         <v>161</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H24" t="s" s="0">
         <v>162</v>
@@ -2550,10 +2427,10 @@
         <v>167</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="H25" t="s" s="0">
         <v>168</v>
@@ -2588,7 +2465,7 @@
         <v>13</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>78</v>
+        <v>13</v>
       </c>
       <c r="H26" t="s" s="0">
         <v>174</v>
@@ -2623,7 +2500,7 @@
         <v>37</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="H27" t="s" s="0">
         <v>180</v>
@@ -2655,7 +2532,7 @@
         <v>185</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G28" t="s" s="0">
         <v>13</v>
@@ -2693,7 +2570,7 @@
         <v>37</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>13</v>
+        <v>72</v>
       </c>
       <c r="H29" t="s" s="0">
         <v>192</v>
@@ -2728,27 +2605,27 @@
         <v>37</v>
       </c>
       <c r="G30" t="s" s="0">
-        <v>13</v>
+        <v>198</v>
       </c>
       <c r="H30" t="s" s="0">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I30" t="s" s="0">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J30" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K30" t="s" s="0">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C31" t="s" s="0">
         <v>2</v>
@@ -2757,33 +2634,33 @@
         <v>3</v>
       </c>
       <c r="E31" t="s" s="0">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F31" t="s" s="0">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="G31" t="s" s="0">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="H31" t="s" s="0">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I31" t="s" s="0">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J31" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K31" t="s" s="0">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s" s="0">
         <v>2</v>
@@ -2792,13 +2669,13 @@
         <v>3</v>
       </c>
       <c r="E32" t="s" s="0">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F32" t="s" s="0">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="G32" t="s" s="0">
-        <v>210</v>
+        <v>72</v>
       </c>
       <c r="H32" t="s" s="0">
         <v>211</v>
@@ -2830,10 +2707,10 @@
         <v>216</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G33" t="s" s="0">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="H33" t="s" s="0">
         <v>217</v>
@@ -2865,30 +2742,30 @@
         <v>222</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="G34" t="s" s="0">
-        <v>78</v>
+        <v>223</v>
       </c>
       <c r="H34" t="s" s="0">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I34" t="s" s="0">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J34" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K34" t="s" s="0">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>2</v>
@@ -2897,33 +2774,33 @@
         <v>3</v>
       </c>
       <c r="E35" t="s" s="0">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F35" t="s" s="0">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H35" t="s" s="0">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I35" t="s" s="0">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="J35" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K35" t="s" s="0">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C36" t="s" s="0">
         <v>2</v>
@@ -2932,13 +2809,13 @@
         <v>3</v>
       </c>
       <c r="E36" t="s" s="0">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F36" t="s" s="0">
         <v>37</v>
       </c>
       <c r="G36" t="s" s="0">
-        <v>235</v>
+        <v>72</v>
       </c>
       <c r="H36" t="s" s="0">
         <v>236</v>
@@ -2970,10 +2847,10 @@
         <v>241</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>111</v>
+        <v>37</v>
       </c>
       <c r="G37" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H37" t="s" s="0">
         <v>242</v>
@@ -3005,10 +2882,10 @@
         <v>247</v>
       </c>
       <c r="F38" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="G38" t="s" s="0">
-        <v>78</v>
       </c>
       <c r="H38" t="s" s="0">
         <v>248</v>
@@ -3040,30 +2917,30 @@
         <v>253</v>
       </c>
       <c r="F39" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G39" t="s" s="0">
-        <v>137</v>
+        <v>254</v>
       </c>
       <c r="H39" t="s" s="0">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I39" t="s" s="0">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J39" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K39" t="s" s="0">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C40" t="s" s="0">
         <v>2</v>
@@ -3072,33 +2949,33 @@
         <v>3</v>
       </c>
       <c r="E40" t="s" s="0">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F40" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G40" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H40" t="s" s="0">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I40" t="s" s="0">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J40" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K40" t="s" s="0">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C41" t="s" s="0">
         <v>2</v>
@@ -3107,33 +2984,33 @@
         <v>3</v>
       </c>
       <c r="E41" t="s" s="0">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F41" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G41" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G41" t="s" s="0">
-        <v>65</v>
-      </c>
       <c r="H41" t="s" s="0">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I41" t="s" s="0">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="J41" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K41" t="s" s="0">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C42" t="s" s="0">
         <v>2</v>
@@ -3142,33 +3019,33 @@
         <v>3</v>
       </c>
       <c r="E42" t="s" s="0">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>37</v>
+        <v>254</v>
       </c>
       <c r="H42" t="s" s="0">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="I42" t="s" s="0">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="J42" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K42" t="s" s="0">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C43" t="s" s="0">
         <v>2</v>
@@ -3177,13 +3054,13 @@
         <v>3</v>
       </c>
       <c r="E43" t="s" s="0">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F43" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G43" t="s" s="0">
-        <v>278</v>
+        <v>72</v>
       </c>
       <c r="H43" t="s" s="0">
         <v>279</v>
@@ -3215,10 +3092,10 @@
         <v>284</v>
       </c>
       <c r="F44" t="s" s="0">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H44" t="s" s="0">
         <v>285</v>
@@ -3250,10 +3127,10 @@
         <v>290</v>
       </c>
       <c r="F45" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G45" t="s" s="0">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="H45" t="s" s="0">
         <v>291</v>
@@ -3285,10 +3162,10 @@
         <v>296</v>
       </c>
       <c r="F46" t="s" s="0">
-        <v>13</v>
+        <v>99</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>278</v>
+        <v>72</v>
       </c>
       <c r="H46" t="s" s="0">
         <v>297</v>
@@ -3323,7 +3200,7 @@
         <v>13</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H47" t="s" s="0">
         <v>303</v>
@@ -3355,10 +3232,10 @@
         <v>308</v>
       </c>
       <c r="F48" t="s" s="0">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H48" t="s" s="0">
         <v>309</v>
@@ -3371,146 +3248,6 @@
       </c>
       <c r="K48" t="s" s="0">
         <v>311</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
-        <v>312</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="C49" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D49" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E49" t="s" s="0">
-        <v>314</v>
-      </c>
-      <c r="F49" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G49" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="H49" t="s" s="0">
-        <v>315</v>
-      </c>
-      <c r="I49" t="s" s="0">
-        <v>316</v>
-      </c>
-      <c r="J49" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K49" t="s" s="0">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
-        <v>318</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>319</v>
-      </c>
-      <c r="C50" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D50" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E50" t="s" s="0">
-        <v>320</v>
-      </c>
-      <c r="F50" t="s" s="0">
-        <v>111</v>
-      </c>
-      <c r="G50" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="H50" t="s" s="0">
-        <v>321</v>
-      </c>
-      <c r="I50" t="s" s="0">
-        <v>322</v>
-      </c>
-      <c r="J50" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K50" t="s" s="0">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B51" t="s" s="0">
-        <v>325</v>
-      </c>
-      <c r="C51" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D51" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E51" t="s" s="0">
-        <v>326</v>
-      </c>
-      <c r="F51" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G51" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="H51" t="s" s="0">
-        <v>327</v>
-      </c>
-      <c r="I51" t="s" s="0">
-        <v>328</v>
-      </c>
-      <c r="J51" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K51" t="s" s="0">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="0">
-        <v>330</v>
-      </c>
-      <c r="B52" t="s" s="0">
-        <v>331</v>
-      </c>
-      <c r="C52" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D52" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E52" t="s" s="0">
-        <v>332</v>
-      </c>
-      <c r="F52" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G52" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="H52" t="s" s="0">
-        <v>333</v>
-      </c>
-      <c r="I52" t="s" s="0">
-        <v>334</v>
-      </c>
-      <c r="J52" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K52" t="s" s="0">
-        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create seperate method and excel file to handle allergy
</commit_message>
<xml_diff>
--- a/recipe.xlsx
+++ b/recipe.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="336">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -158,6 +158,42 @@
     <t>https://www.tarladalal.com/chana-tuvar-and-green-moong-dal-trevati-dal-38470r</t>
   </si>
   <si>
+    <t>Recipe# 40603</t>
+  </si>
+  <si>
+    <t>Baingan Bhaja, Bengali Begun Bhaja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18 big brinjal (baingan / eggplant) slices    2 tsp chilli powder    1/2 tsp turmeric powder (haldi)    1 tbsp lemon juice    1/4 cup besan (bengal gram flour)    salt to taste    2 tsp oil for greasing and cooking    </t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>20 mins</t>
+  </si>
+  <si>
+    <t>, For baingan bhaja
+To make baingan bhaja, combine the chilli powder, turmeric powder, lemon juice, besan, salt and 2 tbsp of water in a deep bowl and mix well.
+Add the baingan slices and mix well. Keep aside.
+Heat a non-stick tava (griddle), grease it with ½ tsp of oil, arrange half the baingan slices and cook using ½ tsp of oil on both the sides till golden brown in colour.
+Repeat step 3 to make 1 more batch.
+Serve the baingan bhaja immediately.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 43 cal
+Protein 1.5 g
+Carbohydrates 4.6 g
+Fiber 3 g
+Fat 2.1 g
+Cholesterol 0 mg
+Sodium 4.3 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/baingan-bhaja-bengali-begun-bhaja-40603r</t>
+  </si>
+  <si>
     <t>Recipe# 5292</t>
   </si>
   <si>
@@ -165,9 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">3/4 cup toovar (arhar) dal    1/4 cup chana dal (split bengal gram)    1 cup chopped tomatoes    2 cups bottle gourd (doodhi / lauki) , cut into big pieces    1/4 tsp turmeric powder (haldi)    1 tsp cumin seeds (jeera)    1/2 tsp chopped garlic (lehsun)    1 tsp chopped green chillies    1 tsp grated ginger (adrak)    3/4 cup sliced onions    2 tsp oil    salt to taste    2 tbsp chopped coriander (dhania)    </t>
-  </si>
-  <si>
-    <t>10 mins</t>
   </si>
   <si>
     <t>25 mins</t>
@@ -301,9 +334,6 @@
     <t xml:space="preserve">3/4 cup brown rice    salt to taste    </t>
   </si>
   <si>
-    <t>20 mins</t>
-  </si>
-  <si>
     <t>, How to cook brown rice
 To cook brown rice, soak the brown rice in enough water for 30 minutes and drain well.
 Combine the brown rice along with 2 cups of water in a pressure cooker and pressure cook for 7 whistles.
@@ -387,6 +417,35 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/masoor-dal-easy-masoor-dal-recipe-40586r</t>
+  </si>
+  <si>
+    <t>Recipe# 7468</t>
+  </si>
+  <si>
+    <t>Fenugreek and Mushroom Brown Rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 cups finely chopped fenugreek (methi) leaves    1 cup sliced mushrooms (khumbh)    1 cup brown rice    2 tsp oil    2 tsp finely chopped green chillies    1 tsp finely chopped ginger (adrak)    1 tbsp finely chopped garlic (lehsun)    1 cup finely chopped onions    1/2 cup finely chopped tomatoes    1/2 cup brinjal (baingan / eggplant) cubes    1/2 cup surti papdi seeds (fresh vaal seeds)    1/2 tsp chilli powder    salt to taste    2 tbsp finely chopped coriander (dhania)    </t>
+  </si>
+  <si>
+    <t>, Heat the oil in a pressure cooker, add the green chillies, ginger, garlic, and onions and sauté on a medium flame for 2 minutes.
+Add the fenugreek leaves, mushrooms, tomatoes, brinjals, surti papadi seeds,and chilli powder, mix well and cook on a medium flame for 1 to 2 minutes, while stirring occasionally.
+Add the brown rice, 2¼ cups of hot water and salt, mix well and pressure cook for 4 whistles.
+Allow the steam to escape before opening the lid.
+Serve hot garnished with coriander.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 151 cal
+Protein 3.9 g
+Carbohydrates 27.6 g
+Fiber 3.3 g
+Fat 2.8 g
+Cholesterol 0 mg
+Sodium 19.9 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/fenugreek-and-mushroom-brown-rice-7468r</t>
   </si>
   <si>
     <t>Recipe# 22173</t>
@@ -1175,6 +1234,40 @@
     <t>https://www.tarladalal.com/apple-magic-lemony-apple-juice-6213r</t>
   </si>
   <si>
+    <t>Recipe# 22206</t>
+  </si>
+  <si>
+    <t>Bhindi Masala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 tender ladies finger (bhindi)    2 tbsp besan (bengal gram flour)    2 tsp oil    1/2 cup roughly chopped onions    1 cup chopped coriander (dhania)    2 tsp ginger-green chilli paste    1/2 tsp turmeric powder (haldi)    1 tbsp coriander-cumin seeds (dhania-jeera) powder    1 tsp garam masala    2 tsp roasted sesame seeds (til)    1 tbsp lemon juice    salt to taste    rotis/parathas    </t>
+  </si>
+  <si>
+    <t>, For the bhindi masala paste
+Combine all the ingredients and 2 tbsp of water in a mixer and blend till smooth.
+Transfer the mixture into a deep bowl, add the besan and mix well. Keep aside.
+How to proceed to make bhindi masala
+To make bhindi masala, wash, dry and slit the bhindi lengthwise.
+Stuff each bhindi with a little prepared paste. Keep the remaining paste aside.
+Heat a non-stick tava (griddle), put the remaining paste and 2 tbsp of water and sauté on a medium flame for 2 minutes.
+Add the stuffed bhindis and sauté on a medium flame for 4 minutes.
+Cover with a lid and cook on a medium flame for 6 to 8 minutes, while stirring occasionally.
+Serve the bhindi masala hot with rotis or parathas.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per serving
+Energy 83 cal
+Protein 3.6 g
+Carbohydrates 14.2 g
+Fiber 3.6 g
+Fat 1.4 g
+Cholesterol 0 mg
+Sodium 15.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/bhindi-masala-22206r</t>
+  </si>
+  <si>
     <t>Recipe# 8651</t>
   </si>
   <si>
@@ -1199,6 +1292,36 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/avocado-dip-avocado-jain-dip-8651r</t>
+  </si>
+  <si>
+    <t>Recipe# 38954</t>
+  </si>
+  <si>
+    <t>Fluffy Egg White Masala Omelette</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 eggs whites    1 tsp olive oil    salt and freshly ground to taste    1/4 cup finely chopped onions    1/2 cup red and yellow capsicum chopped    1/4 cup finely chopped mushrooms (khumbh)    1/4 cup finely chopped tomatoes    1/2 tsp finely chopped green chillies    1 tsp olive oil    </t>
+  </si>
+  <si>
+    <t>, For the masala vegetables
+In a pan, heat the olive oil and sauté the onions, capsicums , mushrooms, and green chilli for 1 minute. Add the tomatoes and cook again. Keep aside.
+How to proceed
+Beat the egg whites in a electric beater on a slow for 2 to 3 minutes or until the mixture is thick and frothy.
+Heat the olive oil in a 10 inch pan. Add the beaten egg and cook for a few minutes checking with a spatula to see when the bottom of the egg is done. Then add the cooked masala vegetables in the centre of the omelette. Fold the omelette into half and serve hot with a whole wheat toast.
+Sprinkle fresh pepper on top.</t>
+  </si>
+  <si>
+    <t>Nutrient values (Abbrv) per omeleltte
+Energy 394 cal
+Protein 22 g
+Carbohydrates 8.9 g
+Fiber 2.6 g
+Fat 30.3 g
+Cholesterol 0 mg
+Sodium 9.4 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/fluffy-egg-white-masala-omelette-38954r</t>
   </si>
   <si>
     <t>Recipe# 39688</t>
@@ -1567,7 +1690,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1762,10 +1885,10 @@
         <v>44</v>
       </c>
       <c r="F6" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s" s="0">
         <v>45</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>13</v>
       </c>
       <c r="H6" t="s" s="0">
         <v>46</v>
@@ -1797,30 +1920,30 @@
         <v>51</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J7" t="s" s="0">
         <v>17</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s" s="0">
         <v>2</v>
@@ -1829,13 +1952,13 @@
         <v>3</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="H8" t="s" s="0">
         <v>59</v>
@@ -1867,7 +1990,7 @@
         <v>64</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="G9" t="s" s="0">
         <v>65</v>
@@ -1902,45 +2025,45 @@
         <v>71</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="G10" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H10" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="H10" t="s" s="0">
+      <c r="I10" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="I10" t="s" s="0">
+      <c r="J10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K10" t="s" s="0">
         <v>74</v>
-      </c>
-      <c r="J10" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K10" t="s" s="0">
-        <v>75</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="B11" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="B11" t="s" s="0">
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="C11" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s" s="0">
+      <c r="F11" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s" s="0">
         <v>78</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s" s="0">
-        <v>65</v>
       </c>
       <c r="H11" t="s" s="0">
         <v>79</v>
@@ -1972,290 +2095,290 @@
         <v>84</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H12" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="H12" t="s" s="0">
+      <c r="I12" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="I12" t="s" s="0">
+      <c r="J12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s" s="0">
         <v>87</v>
-      </c>
-      <c r="J12" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K12" t="s" s="0">
-        <v>88</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="C13" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="C13" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E13" t="s" s="0">
+      <c r="F13" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="H13" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="F13" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G13" t="s" s="0">
+      <c r="I13" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="H13" t="s" s="0">
+      <c r="J13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K13" t="s" s="0">
         <v>93</v>
-      </c>
-      <c r="I13" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="J13" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K13" t="s" s="0">
-        <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="F14" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="C14" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s" s="0">
+      <c r="H14" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="F14" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G14" t="s" s="0">
+      <c r="I14" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="H14" t="s" s="0">
+      <c r="J14" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K14" t="s" s="0">
         <v>100</v>
-      </c>
-      <c r="I14" t="s" s="0">
-        <v>101</v>
-      </c>
-      <c r="J14" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K14" t="s" s="0">
-        <v>102</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s" s="0">
         <v>103</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>104</v>
-      </c>
-      <c r="C15" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D15" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s" s="0">
-        <v>105</v>
       </c>
       <c r="F15" t="s" s="0">
         <v>37</v>
       </c>
       <c r="G15" t="s" s="0">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="H15" t="s" s="0">
+        <v>105</v>
+      </c>
+      <c r="I15" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="I15" t="s" s="0">
+      <c r="J15" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K15" t="s" s="0">
         <v>107</v>
-      </c>
-      <c r="J15" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K15" t="s" s="0">
-        <v>108</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="C16" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="C16" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E16" t="s" s="0">
+      <c r="F16" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G16" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="F16" t="s" s="0">
+      <c r="H16" t="s" s="0">
         <v>112</v>
       </c>
-      <c r="G16" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="H16" t="s" s="0">
+      <c r="I16" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="I16" t="s" s="0">
+      <c r="J16" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K16" t="s" s="0">
         <v>114</v>
-      </c>
-      <c r="J16" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K16" t="s" s="0">
-        <v>115</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
+        <v>115</v>
+      </c>
+      <c r="B17" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="C17" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="C17" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s" s="0">
+      <c r="F17" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H17" t="s" s="0">
         <v>118</v>
       </c>
-      <c r="F17" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G17" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H17" t="s" s="0">
+      <c r="I17" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="I17" t="s" s="0">
+      <c r="J17" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K17" t="s" s="0">
         <v>120</v>
-      </c>
-      <c r="J17" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K17" t="s" s="0">
-        <v>121</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
+        <v>121</v>
+      </c>
+      <c r="B18" t="s" s="0">
         <v>122</v>
       </c>
-      <c r="B18" t="s" s="0">
+      <c r="C18" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s" s="0">
         <v>123</v>
       </c>
-      <c r="C18" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s" s="0">
+      <c r="F18" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="F18" t="s" s="0">
-        <v>99</v>
-      </c>
       <c r="G18" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s" s="0">
         <v>125</v>
       </c>
-      <c r="H18" t="s" s="0">
+      <c r="I18" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="I18" t="s" s="0">
+      <c r="J18" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K18" t="s" s="0">
         <v>127</v>
-      </c>
-      <c r="J18" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K18" t="s" s="0">
-        <v>128</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
+        <v>128</v>
+      </c>
+      <c r="B19" t="s" s="0">
         <v>129</v>
       </c>
-      <c r="B19" t="s" s="0">
+      <c r="C19" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s" s="0">
         <v>130</v>
       </c>
-      <c r="C19" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E19" t="s" s="0">
+      <c r="F19" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G19" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H19" t="s" s="0">
         <v>131</v>
       </c>
-      <c r="F19" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="G19" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="H19" t="s" s="0">
+      <c r="I19" t="s" s="0">
         <v>132</v>
       </c>
-      <c r="I19" t="s" s="0">
+      <c r="J19" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s" s="0">
         <v>133</v>
-      </c>
-      <c r="J19" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K19" t="s" s="0">
-        <v>134</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s" s="0">
         <v>135</v>
       </c>
-      <c r="B20" t="s" s="0">
+      <c r="C20" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s" s="0">
         <v>136</v>
       </c>
-      <c r="C20" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D20" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E20" t="s" s="0">
+      <c r="F20" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="G20" t="s" s="0">
         <v>137</v>
-      </c>
-      <c r="F20" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="G20" t="s" s="0">
-        <v>13</v>
       </c>
       <c r="H20" t="s" s="0">
         <v>138</v>
@@ -2287,10 +2410,10 @@
         <v>143</v>
       </c>
       <c r="F21" t="s" s="0">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s" s="0">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="H21" t="s" s="0">
         <v>144</v>
@@ -2322,10 +2445,10 @@
         <v>149</v>
       </c>
       <c r="F22" t="s" s="0">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="G22" t="s" s="0">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="H22" t="s" s="0">
         <v>150</v>
@@ -2357,10 +2480,10 @@
         <v>155</v>
       </c>
       <c r="F23" t="s" s="0">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="G23" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H23" t="s" s="0">
         <v>156</v>
@@ -2392,10 +2515,10 @@
         <v>161</v>
       </c>
       <c r="F24" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G24" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s" s="0">
         <v>162</v>
@@ -2427,10 +2550,10 @@
         <v>167</v>
       </c>
       <c r="F25" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G25" t="s" s="0">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="H25" t="s" s="0">
         <v>168</v>
@@ -2465,7 +2588,7 @@
         <v>13</v>
       </c>
       <c r="G26" t="s" s="0">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="H26" t="s" s="0">
         <v>174</v>
@@ -2500,7 +2623,7 @@
         <v>37</v>
       </c>
       <c r="G27" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="H27" t="s" s="0">
         <v>180</v>
@@ -2532,7 +2655,7 @@
         <v>185</v>
       </c>
       <c r="F28" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s" s="0">
         <v>13</v>
@@ -2570,7 +2693,7 @@
         <v>37</v>
       </c>
       <c r="G29" t="s" s="0">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="H29" t="s" s="0">
         <v>192</v>
@@ -2605,77 +2728,77 @@
         <v>37</v>
       </c>
       <c r="G30" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s" s="0">
         <v>198</v>
       </c>
-      <c r="H30" t="s" s="0">
+      <c r="I30" t="s" s="0">
         <v>199</v>
       </c>
-      <c r="I30" t="s" s="0">
+      <c r="J30" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K30" t="s" s="0">
         <v>200</v>
-      </c>
-      <c r="J30" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K30" t="s" s="0">
-        <v>201</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
+        <v>201</v>
+      </c>
+      <c r="B31" t="s" s="0">
         <v>202</v>
       </c>
-      <c r="B31" t="s" s="0">
+      <c r="C31" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s" s="0">
         <v>203</v>
       </c>
-      <c r="C31" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E31" t="s" s="0">
+      <c r="F31" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G31" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H31" t="s" s="0">
         <v>204</v>
       </c>
-      <c r="F31" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="G31" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="H31" t="s" s="0">
+      <c r="I31" t="s" s="0">
         <v>205</v>
       </c>
-      <c r="I31" t="s" s="0">
+      <c r="J31" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K31" t="s" s="0">
         <v>206</v>
-      </c>
-      <c r="J31" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K31" t="s" s="0">
-        <v>207</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
+        <v>207</v>
+      </c>
+      <c r="B32" t="s" s="0">
         <v>208</v>
       </c>
-      <c r="B32" t="s" s="0">
+      <c r="C32" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s" s="0">
         <v>209</v>
       </c>
-      <c r="C32" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D32" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E32" t="s" s="0">
+      <c r="F32" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G32" t="s" s="0">
         <v>210</v>
-      </c>
-      <c r="F32" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="G32" t="s" s="0">
-        <v>72</v>
       </c>
       <c r="H32" t="s" s="0">
         <v>211</v>
@@ -2707,10 +2830,10 @@
         <v>216</v>
       </c>
       <c r="F33" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G33" t="s" s="0">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H33" t="s" s="0">
         <v>217</v>
@@ -2742,80 +2865,80 @@
         <v>222</v>
       </c>
       <c r="F34" t="s" s="0">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="G34" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H34" t="s" s="0">
         <v>223</v>
       </c>
-      <c r="H34" t="s" s="0">
+      <c r="I34" t="s" s="0">
         <v>224</v>
       </c>
-      <c r="I34" t="s" s="0">
+      <c r="J34" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K34" t="s" s="0">
         <v>225</v>
-      </c>
-      <c r="J34" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K34" t="s" s="0">
-        <v>226</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
+        <v>226</v>
+      </c>
+      <c r="B35" t="s" s="0">
         <v>227</v>
       </c>
-      <c r="B35" t="s" s="0">
+      <c r="C35" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s" s="0">
         <v>228</v>
       </c>
-      <c r="C35" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s" s="0">
+      <c r="F35" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G35" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H35" t="s" s="0">
         <v>229</v>
       </c>
-      <c r="F35" t="s" s="0">
-        <v>99</v>
-      </c>
-      <c r="G35" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H35" t="s" s="0">
+      <c r="I35" t="s" s="0">
         <v>230</v>
       </c>
-      <c r="I35" t="s" s="0">
+      <c r="J35" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K35" t="s" s="0">
         <v>231</v>
-      </c>
-      <c r="J35" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K35" t="s" s="0">
-        <v>232</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
+        <v>232</v>
+      </c>
+      <c r="B36" t="s" s="0">
         <v>233</v>
       </c>
-      <c r="B36" t="s" s="0">
+      <c r="C36" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s" s="0">
         <v>234</v>
-      </c>
-      <c r="C36" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D36" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E36" t="s" s="0">
-        <v>235</v>
       </c>
       <c r="F36" t="s" s="0">
         <v>37</v>
       </c>
       <c r="G36" t="s" s="0">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="H36" t="s" s="0">
         <v>236</v>
@@ -2847,10 +2970,10 @@
         <v>241</v>
       </c>
       <c r="F37" t="s" s="0">
-        <v>37</v>
+        <v>111</v>
       </c>
       <c r="G37" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H37" t="s" s="0">
         <v>242</v>
@@ -2882,10 +3005,10 @@
         <v>247</v>
       </c>
       <c r="F38" t="s" s="0">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="G38" t="s" s="0">
-        <v>37</v>
+        <v>78</v>
       </c>
       <c r="H38" t="s" s="0">
         <v>248</v>
@@ -2917,150 +3040,150 @@
         <v>253</v>
       </c>
       <c r="F39" t="s" s="0">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G39" t="s" s="0">
+        <v>137</v>
+      </c>
+      <c r="H39" t="s" s="0">
         <v>254</v>
       </c>
-      <c r="H39" t="s" s="0">
+      <c r="I39" t="s" s="0">
         <v>255</v>
       </c>
-      <c r="I39" t="s" s="0">
+      <c r="J39" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K39" t="s" s="0">
         <v>256</v>
-      </c>
-      <c r="J39" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K39" t="s" s="0">
-        <v>257</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
+        <v>257</v>
+      </c>
+      <c r="B40" t="s" s="0">
         <v>258</v>
       </c>
-      <c r="B40" t="s" s="0">
+      <c r="C40" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s" s="0">
         <v>259</v>
       </c>
-      <c r="C40" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D40" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E40" t="s" s="0">
+      <c r="F40" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G40" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H40" t="s" s="0">
         <v>260</v>
       </c>
-      <c r="F40" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G40" t="s" s="0">
-        <v>72</v>
-      </c>
-      <c r="H40" t="s" s="0">
+      <c r="I40" t="s" s="0">
         <v>261</v>
       </c>
-      <c r="I40" t="s" s="0">
+      <c r="J40" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K40" t="s" s="0">
         <v>262</v>
-      </c>
-      <c r="J40" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K40" t="s" s="0">
-        <v>263</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s" s="0">
+        <v>263</v>
+      </c>
+      <c r="B41" t="s" s="0">
         <v>264</v>
       </c>
-      <c r="B41" t="s" s="0">
+      <c r="C41" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s" s="0">
         <v>265</v>
       </c>
-      <c r="C41" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D41" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E41" t="s" s="0">
+      <c r="F41" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G41" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="H41" t="s" s="0">
         <v>266</v>
       </c>
-      <c r="F41" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G41" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="H41" t="s" s="0">
+      <c r="I41" t="s" s="0">
         <v>267</v>
       </c>
-      <c r="I41" t="s" s="0">
+      <c r="J41" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K41" t="s" s="0">
         <v>268</v>
-      </c>
-      <c r="J41" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K41" t="s" s="0">
-        <v>269</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="0">
+        <v>269</v>
+      </c>
+      <c r="B42" t="s" s="0">
         <v>270</v>
       </c>
-      <c r="B42" t="s" s="0">
+      <c r="C42" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s" s="0">
         <v>271</v>
-      </c>
-      <c r="C42" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D42" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E42" t="s" s="0">
-        <v>272</v>
       </c>
       <c r="F42" t="s" s="0">
         <v>13</v>
       </c>
       <c r="G42" t="s" s="0">
-        <v>254</v>
+        <v>37</v>
       </c>
       <c r="H42" t="s" s="0">
+        <v>272</v>
+      </c>
+      <c r="I42" t="s" s="0">
         <v>273</v>
       </c>
-      <c r="I42" t="s" s="0">
+      <c r="J42" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K42" t="s" s="0">
         <v>274</v>
-      </c>
-      <c r="J42" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="K42" t="s" s="0">
-        <v>275</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="0">
+        <v>275</v>
+      </c>
+      <c r="B43" t="s" s="0">
         <v>276</v>
       </c>
-      <c r="B43" t="s" s="0">
+      <c r="C43" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s" s="0">
         <v>277</v>
       </c>
-      <c r="C43" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="D43" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="E43" t="s" s="0">
+      <c r="F43" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G43" t="s" s="0">
         <v>278</v>
-      </c>
-      <c r="F43" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="G43" t="s" s="0">
-        <v>72</v>
       </c>
       <c r="H43" t="s" s="0">
         <v>279</v>
@@ -3092,10 +3215,10 @@
         <v>284</v>
       </c>
       <c r="F44" t="s" s="0">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="G44" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H44" t="s" s="0">
         <v>285</v>
@@ -3127,10 +3250,10 @@
         <v>290</v>
       </c>
       <c r="F45" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G45" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="G45" t="s" s="0">
-        <v>72</v>
       </c>
       <c r="H45" t="s" s="0">
         <v>291</v>
@@ -3162,10 +3285,10 @@
         <v>296</v>
       </c>
       <c r="F46" t="s" s="0">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="G46" t="s" s="0">
-        <v>72</v>
+        <v>278</v>
       </c>
       <c r="H46" t="s" s="0">
         <v>297</v>
@@ -3200,7 +3323,7 @@
         <v>13</v>
       </c>
       <c r="G47" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H47" t="s" s="0">
         <v>303</v>
@@ -3232,10 +3355,10 @@
         <v>308</v>
       </c>
       <c r="F48" t="s" s="0">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="G48" t="s" s="0">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H48" t="s" s="0">
         <v>309</v>
@@ -3248,6 +3371,146 @@
       </c>
       <c r="K48" t="s" s="0">
         <v>311</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="0">
+        <v>312</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>313</v>
+      </c>
+      <c r="C49" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s" s="0">
+        <v>314</v>
+      </c>
+      <c r="F49" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="G49" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H49" t="s" s="0">
+        <v>315</v>
+      </c>
+      <c r="I49" t="s" s="0">
+        <v>316</v>
+      </c>
+      <c r="J49" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K49" t="s" s="0">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="0">
+        <v>318</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>319</v>
+      </c>
+      <c r="C50" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s" s="0">
+        <v>320</v>
+      </c>
+      <c r="F50" t="s" s="0">
+        <v>111</v>
+      </c>
+      <c r="G50" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H50" t="s" s="0">
+        <v>321</v>
+      </c>
+      <c r="I50" t="s" s="0">
+        <v>322</v>
+      </c>
+      <c r="J50" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K50" t="s" s="0">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="0">
+        <v>324</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>325</v>
+      </c>
+      <c r="C51" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s" s="0">
+        <v>326</v>
+      </c>
+      <c r="F51" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G51" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H51" t="s" s="0">
+        <v>327</v>
+      </c>
+      <c r="I51" t="s" s="0">
+        <v>328</v>
+      </c>
+      <c r="J51" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K51" t="s" s="0">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="0">
+        <v>330</v>
+      </c>
+      <c r="B52" t="s" s="0">
+        <v>331</v>
+      </c>
+      <c r="C52" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s" s="0">
+        <v>332</v>
+      </c>
+      <c r="F52" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="G52" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="H52" t="s" s="0">
+        <v>333</v>
+      </c>
+      <c r="I52" t="s" s="0">
+        <v>334</v>
+      </c>
+      <c r="J52" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="K52" t="s" s="0">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>